<commit_message>
pre-close commit - updated flow processing and added transformation groups for data processing
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F52496-8A62-4644-BFF4-FE8A16AEB13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCEE1E6-9A5B-45CE-BAEC-98E3937AB60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="25812" windowWidth="30936" windowHeight="18696" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="6936" yWindow="25812" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="173">
   <si>
     <t>Plate</t>
   </si>
@@ -531,6 +531,33 @@
   </si>
   <si>
     <t>flo,OD</t>
+  </si>
+  <si>
+    <t>rem_none_samples</t>
+  </si>
+  <si>
+    <t>cat(sg_1_none,sg_2_none,sg_3_none,sg_4_none) .- mean(control_M9_KC)</t>
+  </si>
+  <si>
+    <t>cat(sg_1_atc,sg_2_atc,sg_3_atc,sg_4_atc) .- mean(control_M9_KC_atc)</t>
+  </si>
+  <si>
+    <t>rem_atc_samples</t>
+  </si>
+  <si>
+    <t>rem_IPTG_samples</t>
+  </si>
+  <si>
+    <t>cat(sg_1_IPTG,sg_2_IPTG,sg_3_IPTG,sg_4_IPTG) .- mean(control_M9_KC_IPTG)</t>
+  </si>
+  <si>
+    <t>rem_atc_IPTG_samples</t>
+  </si>
+  <si>
+    <t>cat(sg_1__atc_IPTG,sg_2_atc_IPTG,sg_3_atc_IPTG,sg_4_atc_IPTG) .- mean(control_M9_KC_atc_IPTG)</t>
+  </si>
+  <si>
+    <t>norm_flo</t>
   </si>
 </sst>
 </file>
@@ -910,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2583,7 +2610,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2831,13 +2858,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2845,6 +2875,43 @@
       </c>
       <c r="B1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
broke the code a bit, building it back up
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCEE1E6-9A5B-45CE-BAEC-98E3937AB60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9402C1-C486-4F5A-8C81-629A9C27C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="25812" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="34560" windowHeight="18600" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="222">
   <si>
     <t>Plate</t>
   </si>
@@ -557,7 +557,154 @@
     <t>cat(sg_1__atc_IPTG,sg_2_atc_IPTG,sg_3_atc_IPTG,sg_4_atc_IPTG) .- mean(control_M9_KC_atc_IPTG)</t>
   </si>
   <si>
-    <t>norm_flo</t>
+    <t>cat(rem_none_samples.flo,rem_atc_samples.flo,rem_IPTG_samples.flo,rem_atc_IPTG_samples.flo)</t>
+  </si>
+  <si>
+    <t>combine_samples</t>
+  </si>
+  <si>
+    <t>rem_single</t>
+  </si>
+  <si>
+    <t>cat(sg_1,sg_2,sg_3,sg_4) .- mean(control_M9_K)</t>
+  </si>
+  <si>
+    <t>rem_wt</t>
+  </si>
+  <si>
+    <t>wt .- mean(control_M9_NOAB)</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/20191121_beads.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_1.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_2.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_3.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_4.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_5.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_6.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_7.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_8.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_9.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pMed_None_0_10.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_1.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_2.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_3.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_4.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_5.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_6.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_7.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pNeg_None_0_8.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_1.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_2.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_3.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_4.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_5.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_6.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_7.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_8.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_9.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_10.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_11.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pStrong_None_0_12.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_1.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_2.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_3.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_4.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_5.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_7.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_8.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_9.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_10.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_11.fcs</t>
+  </si>
+  <si>
+    <t>/home/micha/flopr-master/examples/flow_cytometry/DATA/20191121/pWeak_None_0_12.fcs</t>
+  </si>
+  <si>
+    <t>FSC-A,SSC-A,BL1-H</t>
   </si>
 </sst>
 </file>
@@ -935,16 +1082,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2597,6 +2744,720 @@
       </c>
       <c r="F97" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>178</v>
+      </c>
+      <c r="E98" t="s">
+        <v>179</v>
+      </c>
+      <c r="F98" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>178</v>
+      </c>
+      <c r="E99" t="s">
+        <v>180</v>
+      </c>
+      <c r="F99" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="B100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" t="s">
+        <v>181</v>
+      </c>
+      <c r="F100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>2</v>
+      </c>
+      <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E101" t="s">
+        <v>182</v>
+      </c>
+      <c r="F101" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>178</v>
+      </c>
+      <c r="E102" t="s">
+        <v>183</v>
+      </c>
+      <c r="F102" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>2</v>
+      </c>
+      <c r="B103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" t="s">
+        <v>178</v>
+      </c>
+      <c r="E103" t="s">
+        <v>184</v>
+      </c>
+      <c r="F103" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>2</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>178</v>
+      </c>
+      <c r="E104" t="s">
+        <v>185</v>
+      </c>
+      <c r="F104" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" t="s">
+        <v>178</v>
+      </c>
+      <c r="E105" t="s">
+        <v>186</v>
+      </c>
+      <c r="F105" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" t="s">
+        <v>178</v>
+      </c>
+      <c r="E106" t="s">
+        <v>187</v>
+      </c>
+      <c r="F106" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>2</v>
+      </c>
+      <c r="B107" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" t="s">
+        <v>178</v>
+      </c>
+      <c r="E107" t="s">
+        <v>188</v>
+      </c>
+      <c r="F107" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
+      <c r="D108" t="s">
+        <v>178</v>
+      </c>
+      <c r="E108" t="s">
+        <v>189</v>
+      </c>
+      <c r="F108" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>2</v>
+      </c>
+      <c r="B109" t="s">
+        <v>17</v>
+      </c>
+      <c r="D109" t="s">
+        <v>178</v>
+      </c>
+      <c r="E109" t="s">
+        <v>190</v>
+      </c>
+      <c r="F109" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>2</v>
+      </c>
+      <c r="B110" t="s">
+        <v>23</v>
+      </c>
+      <c r="D110" t="s">
+        <v>178</v>
+      </c>
+      <c r="E110" t="s">
+        <v>191</v>
+      </c>
+      <c r="F110" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>2</v>
+      </c>
+      <c r="B111" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" t="s">
+        <v>178</v>
+      </c>
+      <c r="E111" t="s">
+        <v>192</v>
+      </c>
+      <c r="F111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>2</v>
+      </c>
+      <c r="B112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" t="s">
+        <v>178</v>
+      </c>
+      <c r="E112" t="s">
+        <v>193</v>
+      </c>
+      <c r="F112" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>2</v>
+      </c>
+      <c r="B113" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" t="s">
+        <v>178</v>
+      </c>
+      <c r="E113" t="s">
+        <v>194</v>
+      </c>
+      <c r="F113" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="D114" t="s">
+        <v>178</v>
+      </c>
+      <c r="E114" t="s">
+        <v>195</v>
+      </c>
+      <c r="F114" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>2</v>
+      </c>
+      <c r="B115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
+        <v>178</v>
+      </c>
+      <c r="E115" t="s">
+        <v>196</v>
+      </c>
+      <c r="F115" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116" t="s">
+        <v>178</v>
+      </c>
+      <c r="E116" t="s">
+        <v>197</v>
+      </c>
+      <c r="F116" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117" t="s">
+        <v>30</v>
+      </c>
+      <c r="D117" t="s">
+        <v>178</v>
+      </c>
+      <c r="E117" t="s">
+        <v>198</v>
+      </c>
+      <c r="F117" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>2</v>
+      </c>
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="D118" t="s">
+        <v>178</v>
+      </c>
+      <c r="E118" t="s">
+        <v>199</v>
+      </c>
+      <c r="F118" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s">
+        <v>178</v>
+      </c>
+      <c r="E119" t="s">
+        <v>200</v>
+      </c>
+      <c r="F119" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120" t="s">
+        <v>33</v>
+      </c>
+      <c r="D120" t="s">
+        <v>178</v>
+      </c>
+      <c r="E120" t="s">
+        <v>201</v>
+      </c>
+      <c r="F120" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>2</v>
+      </c>
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="D121" t="s">
+        <v>178</v>
+      </c>
+      <c r="E121" t="s">
+        <v>202</v>
+      </c>
+      <c r="F121" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>2</v>
+      </c>
+      <c r="B122" t="s">
+        <v>35</v>
+      </c>
+      <c r="D122" t="s">
+        <v>178</v>
+      </c>
+      <c r="E122" t="s">
+        <v>203</v>
+      </c>
+      <c r="F122" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>2</v>
+      </c>
+      <c r="B123" t="s">
+        <v>36</v>
+      </c>
+      <c r="D123" t="s">
+        <v>178</v>
+      </c>
+      <c r="E123" t="s">
+        <v>204</v>
+      </c>
+      <c r="F123" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>2</v>
+      </c>
+      <c r="B124" t="s">
+        <v>37</v>
+      </c>
+      <c r="D124" t="s">
+        <v>178</v>
+      </c>
+      <c r="E124" t="s">
+        <v>205</v>
+      </c>
+      <c r="F124" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>2</v>
+      </c>
+      <c r="B125" t="s">
+        <v>38</v>
+      </c>
+      <c r="D125" t="s">
+        <v>178</v>
+      </c>
+      <c r="E125" t="s">
+        <v>206</v>
+      </c>
+      <c r="F125" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>2</v>
+      </c>
+      <c r="B126" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126" t="s">
+        <v>178</v>
+      </c>
+      <c r="E126" t="s">
+        <v>207</v>
+      </c>
+      <c r="F126" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127" t="s">
+        <v>40</v>
+      </c>
+      <c r="D127" t="s">
+        <v>178</v>
+      </c>
+      <c r="E127" t="s">
+        <v>208</v>
+      </c>
+      <c r="F127" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128" t="s">
+        <v>41</v>
+      </c>
+      <c r="D128" t="s">
+        <v>178</v>
+      </c>
+      <c r="E128" t="s">
+        <v>209</v>
+      </c>
+      <c r="F128" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>2</v>
+      </c>
+      <c r="B129" t="s">
+        <v>42</v>
+      </c>
+      <c r="D129" t="s">
+        <v>178</v>
+      </c>
+      <c r="E129" t="s">
+        <v>210</v>
+      </c>
+      <c r="F129" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130" t="s">
+        <v>43</v>
+      </c>
+      <c r="D130" t="s">
+        <v>178</v>
+      </c>
+      <c r="E130" t="s">
+        <v>211</v>
+      </c>
+      <c r="F130" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>2</v>
+      </c>
+      <c r="B131" t="s">
+        <v>44</v>
+      </c>
+      <c r="D131" t="s">
+        <v>178</v>
+      </c>
+      <c r="E131" t="s">
+        <v>212</v>
+      </c>
+      <c r="F131" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>2</v>
+      </c>
+      <c r="B132" t="s">
+        <v>45</v>
+      </c>
+      <c r="D132" t="s">
+        <v>178</v>
+      </c>
+      <c r="E132" t="s">
+        <v>213</v>
+      </c>
+      <c r="F132" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>2</v>
+      </c>
+      <c r="B133" t="s">
+        <v>46</v>
+      </c>
+      <c r="D133" t="s">
+        <v>178</v>
+      </c>
+      <c r="E133" t="s">
+        <v>214</v>
+      </c>
+      <c r="F133" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>2</v>
+      </c>
+      <c r="B134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D134" t="s">
+        <v>178</v>
+      </c>
+      <c r="E134" t="s">
+        <v>215</v>
+      </c>
+      <c r="F134" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135" t="s">
+        <v>49</v>
+      </c>
+      <c r="D135" t="s">
+        <v>178</v>
+      </c>
+      <c r="E135" t="s">
+        <v>216</v>
+      </c>
+      <c r="F135" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136" t="s">
+        <v>50</v>
+      </c>
+      <c r="D136" t="s">
+        <v>178</v>
+      </c>
+      <c r="E136" t="s">
+        <v>217</v>
+      </c>
+      <c r="F136" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137" t="s">
+        <v>51</v>
+      </c>
+      <c r="D137" t="s">
+        <v>178</v>
+      </c>
+      <c r="E137" t="s">
+        <v>218</v>
+      </c>
+      <c r="F137" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138" t="s">
+        <v>52</v>
+      </c>
+      <c r="D138" t="s">
+        <v>178</v>
+      </c>
+      <c r="E138" t="s">
+        <v>219</v>
+      </c>
+      <c r="F138" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>2</v>
+      </c>
+      <c r="B139" t="s">
+        <v>53</v>
+      </c>
+      <c r="D139" t="s">
+        <v>178</v>
+      </c>
+      <c r="E139" t="s">
+        <v>220</v>
+      </c>
+      <c r="F139" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2610,7 +3471,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2858,10 +3719,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2911,6 +3772,25 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more changes to the equation reading stuff
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9402C1-C486-4F5A-8C81-629A9C27C08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2F1D1-8A86-4704-9B46-A2F5DE83B612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="34560" windowHeight="18600" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="6936" yWindow="25812" windowWidth="30936" windowHeight="18696" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="223">
   <si>
     <t>Plate</t>
   </si>
@@ -536,39 +536,21 @@
     <t>rem_none_samples</t>
   </si>
   <si>
-    <t>cat(sg_1_none,sg_2_none,sg_3_none,sg_4_none) .- mean(control_M9_KC)</t>
-  </si>
-  <si>
-    <t>cat(sg_1_atc,sg_2_atc,sg_3_atc,sg_4_atc) .- mean(control_M9_KC_atc)</t>
-  </si>
-  <si>
     <t>rem_atc_samples</t>
   </si>
   <si>
     <t>rem_IPTG_samples</t>
   </si>
   <si>
-    <t>cat(sg_1_IPTG,sg_2_IPTG,sg_3_IPTG,sg_4_IPTG) .- mean(control_M9_KC_IPTG)</t>
-  </si>
-  <si>
     <t>rem_atc_IPTG_samples</t>
   </si>
   <si>
-    <t>cat(sg_1__atc_IPTG,sg_2_atc_IPTG,sg_3_atc_IPTG,sg_4_atc_IPTG) .- mean(control_M9_KC_atc_IPTG)</t>
-  </si>
-  <si>
-    <t>cat(rem_none_samples.flo,rem_atc_samples.flo,rem_IPTG_samples.flo,rem_atc_IPTG_samples.flo)</t>
-  </si>
-  <si>
     <t>combine_samples</t>
   </si>
   <si>
     <t>rem_single</t>
   </si>
   <si>
-    <t>cat(sg_1,sg_2,sg_3,sg_4) .- mean(control_M9_K)</t>
-  </si>
-  <si>
     <t>rem_wt</t>
   </si>
   <si>
@@ -705,6 +687,27 @@
   </si>
   <si>
     <t>FSC-A,SSC-A,BL1-H</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_none,sg_2_none,sg_3_none,sg_4_none) .- mean(control_M9_KC)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc,sg_2_atc,sg_3_atc,sg_4_atc) .- mean(control_M9_KC_atc)</t>
+  </si>
+  <si>
+    <t>hcat(rem_none_samples.flo,rem_atc_samples.flo,rem_IPTG_samples.flo,rem_atc_IPTG_samples.flo)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_iptg,sg_2_iptg,sg_3_iptg,sg_4_iptg) .- mean(control_M9_KC_IPTG)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc_iptg,sg_2_atc_iptg,sg_3_atc_iptg,sg_4_atc_iptg) .- mean(control_M9_KC_atc_IPTG)</t>
+  </si>
+  <si>
+    <t>hcat(sg1,sg2,sg3,sg4) .- mean(control_M9_K)</t>
+  </si>
+  <si>
+    <t>comb</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="A134" sqref="A134:XFD139"/>
     </sheetView>
   </sheetViews>
@@ -2754,13 +2757,13 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E98" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F98" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2771,13 +2774,13 @@
         <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E99" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F99" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2788,13 +2791,13 @@
         <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E100" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F100" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2805,13 +2808,13 @@
         <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E101" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F101" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2822,13 +2825,13 @@
         <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E102" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F102" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2839,13 +2842,13 @@
         <v>11</v>
       </c>
       <c r="D103" t="s">
+        <v>172</v>
+      </c>
+      <c r="E103" t="s">
         <v>178</v>
       </c>
-      <c r="E103" t="s">
-        <v>184</v>
-      </c>
       <c r="F103" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2856,13 +2859,13 @@
         <v>12</v>
       </c>
       <c r="D104" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E104" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F104" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2873,13 +2876,13 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E105" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F105" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2890,13 +2893,13 @@
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E106" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F106" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2907,13 +2910,13 @@
         <v>15</v>
       </c>
       <c r="D107" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E107" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F107" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2924,13 +2927,13 @@
         <v>16</v>
       </c>
       <c r="D108" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E108" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F108" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2941,13 +2944,13 @@
         <v>17</v>
       </c>
       <c r="D109" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E109" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F109" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2958,13 +2961,13 @@
         <v>23</v>
       </c>
       <c r="D110" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E110" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F110" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2975,13 +2978,13 @@
         <v>24</v>
       </c>
       <c r="D111" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E111" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F111" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2992,13 +2995,13 @@
         <v>25</v>
       </c>
       <c r="D112" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E112" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F112" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3009,13 +3012,13 @@
         <v>26</v>
       </c>
       <c r="D113" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E113" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F113" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3026,13 +3029,13 @@
         <v>27</v>
       </c>
       <c r="D114" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E114" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F114" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3043,13 +3046,13 @@
         <v>28</v>
       </c>
       <c r="D115" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E115" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F115" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3060,13 +3063,13 @@
         <v>29</v>
       </c>
       <c r="D116" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E116" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F116" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3077,13 +3080,13 @@
         <v>30</v>
       </c>
       <c r="D117" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E117" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F117" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3094,13 +3097,13 @@
         <v>31</v>
       </c>
       <c r="D118" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E118" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F118" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3111,13 +3114,13 @@
         <v>32</v>
       </c>
       <c r="D119" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E119" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F119" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3128,13 +3131,13 @@
         <v>33</v>
       </c>
       <c r="D120" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E120" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F120" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3145,13 +3148,13 @@
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E121" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F121" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3162,13 +3165,13 @@
         <v>35</v>
       </c>
       <c r="D122" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E122" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F122" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3179,13 +3182,13 @@
         <v>36</v>
       </c>
       <c r="D123" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E123" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F123" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3196,13 +3199,13 @@
         <v>37</v>
       </c>
       <c r="D124" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E124" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F124" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3213,13 +3216,13 @@
         <v>38</v>
       </c>
       <c r="D125" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E125" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F125" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,13 +3233,13 @@
         <v>39</v>
       </c>
       <c r="D126" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E126" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F126" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3247,13 +3250,13 @@
         <v>40</v>
       </c>
       <c r="D127" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E127" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F127" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3264,13 +3267,13 @@
         <v>41</v>
       </c>
       <c r="D128" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E128" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F128" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3281,13 +3284,13 @@
         <v>42</v>
       </c>
       <c r="D129" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E129" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F129" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3298,13 +3301,13 @@
         <v>43</v>
       </c>
       <c r="D130" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E130" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F130" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3315,13 +3318,13 @@
         <v>44</v>
       </c>
       <c r="D131" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E131" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F131" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3332,13 +3335,13 @@
         <v>45</v>
       </c>
       <c r="D132" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E132" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F132" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,13 +3352,13 @@
         <v>46</v>
       </c>
       <c r="D133" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E133" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F133" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3366,13 +3369,13 @@
         <v>48</v>
       </c>
       <c r="D134" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E134" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F134" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3383,13 +3386,13 @@
         <v>49</v>
       </c>
       <c r="D135" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E135" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F135" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3400,13 +3403,13 @@
         <v>50</v>
       </c>
       <c r="D136" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E136" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F136" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3417,13 +3420,13 @@
         <v>51</v>
       </c>
       <c r="D137" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E137" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F137" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3434,13 +3437,13 @@
         <v>52</v>
       </c>
       <c r="D138" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E138" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F138" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3451,13 +3454,13 @@
         <v>53</v>
       </c>
       <c r="D139" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E139" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F139" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3471,7 +3474,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3719,7 +3722,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -3743,55 +3746,55 @@
         <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3801,10 +3804,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3817,6 +3820,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some late night fixes
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2F1D1-8A86-4704-9B46-A2F5DE83B612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E96DD8-CAA0-4F7C-8CBE-6FD2224B1A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="25812" windowWidth="30936" windowHeight="18696" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="224">
   <si>
     <t>Plate</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>comb</t>
+  </si>
+  <si>
+    <t>combine_samples,plate_01_time.flo</t>
   </si>
 </sst>
 </file>
@@ -3725,7 +3728,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3807,7 +3810,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3825,7 +3828,7 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moslty fixed now. Functions to be added.
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E96DD8-CAA0-4F7C-8CBE-6FD2224B1A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5DD274-DCC3-4F16-81E5-4D2B638B162F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="9348" yWindow="480" windowWidth="34560" windowHeight="18600" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="242">
   <si>
     <t>Plate</t>
   </si>
@@ -533,30 +533,6 @@
     <t>flo,OD</t>
   </si>
   <si>
-    <t>rem_none_samples</t>
-  </si>
-  <si>
-    <t>rem_atc_samples</t>
-  </si>
-  <si>
-    <t>rem_IPTG_samples</t>
-  </si>
-  <si>
-    <t>rem_atc_IPTG_samples</t>
-  </si>
-  <si>
-    <t>combine_samples</t>
-  </si>
-  <si>
-    <t>rem_single</t>
-  </si>
-  <si>
-    <t>rem_wt</t>
-  </si>
-  <si>
-    <t>wt .- mean(control_M9_NOAB)</t>
-  </si>
-  <si>
     <t>Flow</t>
   </si>
   <si>
@@ -689,28 +665,106 @@
     <t>FSC-A,SSC-A,BL1-H</t>
   </si>
   <si>
-    <t>hcat(sg_1_none,sg_2_none,sg_3_none,sg_4_none) .- mean(control_M9_KC)</t>
-  </si>
-  <si>
-    <t>hcat(sg_1_atc,sg_2_atc,sg_3_atc,sg_4_atc) .- mean(control_M9_KC_atc)</t>
-  </si>
-  <si>
-    <t>hcat(rem_none_samples.flo,rem_atc_samples.flo,rem_IPTG_samples.flo,rem_atc_IPTG_samples.flo)</t>
-  </si>
-  <si>
-    <t>hcat(sg_1_iptg,sg_2_iptg,sg_3_iptg,sg_4_iptg) .- mean(control_M9_KC_IPTG)</t>
-  </si>
-  <si>
-    <t>hcat(sg_1_atc_iptg,sg_2_atc_iptg,sg_3_atc_iptg,sg_4_atc_iptg) .- mean(control_M9_KC_atc_IPTG)</t>
-  </si>
-  <si>
-    <t>hcat(sg1,sg2,sg3,sg4) .- mean(control_M9_K)</t>
-  </si>
-  <si>
     <t>comb</t>
   </si>
   <si>
     <t>combine_samples,plate_01_time.flo</t>
+  </si>
+  <si>
+    <t>flo_od</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>rem_none_samples_flo</t>
+  </si>
+  <si>
+    <t>rem_atc_samples_flo</t>
+  </si>
+  <si>
+    <t>rem_IPTG_samples_flo</t>
+  </si>
+  <si>
+    <t>rem_atc_IPTG_samples_flo</t>
+  </si>
+  <si>
+    <t>rem_single_flo</t>
+  </si>
+  <si>
+    <t>rem_wt_flo</t>
+  </si>
+  <si>
+    <t>rem_none_samples_od</t>
+  </si>
+  <si>
+    <t>rem_atc_samples_od</t>
+  </si>
+  <si>
+    <t>rem_IPTG_samples_od</t>
+  </si>
+  <si>
+    <t>rem_atc_IPTG_samples_od</t>
+  </si>
+  <si>
+    <t>rem_single_od</t>
+  </si>
+  <si>
+    <t>rem_wt_od</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_none.flo,sg_2_none.flo,sg_3_none.flo,sg_4_none.flo) .- mean(control_M9_KC.flo)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc.flo,sg_2_atc.flo,sg_3_atc.flo,sg_4_atc.flo) .- mean(control_M9_KC_atc.flo)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_iptg.flo,sg_2_iptg.flo,sg_3_iptg.flo,sg_4_iptg.flo) .- mean(control_M9_KC_IPTG.flo)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc_iptg.flo,sg_2_atc_iptg.flo,sg_3_atc_iptg.flo,sg_4_atc_iptg.flo) .- mean(control_M9_KC_atc_IPTG.flo)</t>
+  </si>
+  <si>
+    <t>hcat(sg1.flo,sg2.flo,sg3.flo,sg4.flo) .- mean(control_M9_K.flo)</t>
+  </si>
+  <si>
+    <t>wt.flo .- mean(control_M9_NOAB.flo)</t>
+  </si>
+  <si>
+    <t>wt.OD .- mean(control_M9_NOAB.OD)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_none.OD,sg_2_none.OD,sg_3_none.OD,sg_4_none.OD) .- mean(control_M9_KC.OD)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc.OD,sg_2_atc.OD,sg_3_atc.OD,sg_4_atc.OD) .- mean(control_M9_KC_atc.OD)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_iptg.OD,sg_2_iptg.OD,sg_3_iptg.OD,sg_4_iptg.OD) .- mean(control_M9_KC_IPTG.OD)</t>
+  </si>
+  <si>
+    <t>hcat(sg_1_atc_iptg.OD,sg_2_atc_iptg.OD,sg_3_atc_iptg.OD,sg_4_atc_iptg.OD) .- mean(control_M9_KC_atc_IPTG.OD)</t>
+  </si>
+  <si>
+    <t>hcat(sg1.OD,sg2.OD,sg3.OD,sg4.OD) .- mean(control_M9_K.OD)</t>
+  </si>
+  <si>
+    <t>combine_samples_flo</t>
+  </si>
+  <si>
+    <t>combine_samples_od</t>
+  </si>
+  <si>
+    <t>hcat(rem_none_samples_od,rem_atc_samples_od,rem_IPTG_samples_od,rem_atc_IPTG_samples_od,rem_wt_od,rem_single_od)</t>
+  </si>
+  <si>
+    <t>(combine_samples_flo ./ combine_samples_od)</t>
+  </si>
+  <si>
+    <t>hcat(rem_none_samples_flo,rem_atc_samples_flo,rem_IPTG_samples_flo,rem_atc_IPTG_samples_flo,rem_wt_flo,rem_single_flo)</t>
+  </si>
+  <si>
+    <t>plate_01_time.flo,flo_od</t>
   </si>
 </sst>
 </file>
@@ -2760,13 +2814,13 @@
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E98" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F98" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2777,13 +2831,13 @@
         <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E99" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F99" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2794,13 +2848,13 @@
         <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E100" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F100" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2811,13 +2865,13 @@
         <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E101" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F101" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2828,13 +2882,13 @@
         <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E102" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F102" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -2845,13 +2899,13 @@
         <v>11</v>
       </c>
       <c r="D103" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E103" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F103" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -2862,13 +2916,13 @@
         <v>12</v>
       </c>
       <c r="D104" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E104" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F104" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -2879,13 +2933,13 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
+        <v>164</v>
+      </c>
+      <c r="E105" t="s">
         <v>172</v>
       </c>
-      <c r="E105" t="s">
-        <v>180</v>
-      </c>
       <c r="F105" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -2896,13 +2950,13 @@
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E106" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F106" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -2913,13 +2967,13 @@
         <v>15</v>
       </c>
       <c r="D107" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E107" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F107" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -2930,13 +2984,13 @@
         <v>16</v>
       </c>
       <c r="D108" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E108" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F108" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -2947,13 +3001,13 @@
         <v>17</v>
       </c>
       <c r="D109" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E109" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F109" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -2964,13 +3018,13 @@
         <v>23</v>
       </c>
       <c r="D110" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E110" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F110" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -2981,13 +3035,13 @@
         <v>24</v>
       </c>
       <c r="D111" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E111" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F111" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -2998,13 +3052,13 @@
         <v>25</v>
       </c>
       <c r="D112" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E112" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="F112" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -3015,13 +3069,13 @@
         <v>26</v>
       </c>
       <c r="D113" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E113" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F113" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -3032,13 +3086,13 @@
         <v>27</v>
       </c>
       <c r="D114" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E114" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F114" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -3049,13 +3103,13 @@
         <v>28</v>
       </c>
       <c r="D115" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E115" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F115" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -3066,13 +3120,13 @@
         <v>29</v>
       </c>
       <c r="D116" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E116" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F116" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -3083,13 +3137,13 @@
         <v>30</v>
       </c>
       <c r="D117" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E117" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F117" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -3100,13 +3154,13 @@
         <v>31</v>
       </c>
       <c r="D118" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E118" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F118" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,13 +3171,13 @@
         <v>32</v>
       </c>
       <c r="D119" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E119" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F119" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -3134,13 +3188,13 @@
         <v>33</v>
       </c>
       <c r="D120" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E120" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F120" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -3151,13 +3205,13 @@
         <v>34</v>
       </c>
       <c r="D121" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E121" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F121" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -3168,13 +3222,13 @@
         <v>35</v>
       </c>
       <c r="D122" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E122" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F122" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -3185,13 +3239,13 @@
         <v>36</v>
       </c>
       <c r="D123" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E123" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F123" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -3202,13 +3256,13 @@
         <v>37</v>
       </c>
       <c r="D124" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E124" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F124" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -3219,13 +3273,13 @@
         <v>38</v>
       </c>
       <c r="D125" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E125" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F125" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -3236,13 +3290,13 @@
         <v>39</v>
       </c>
       <c r="D126" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E126" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F126" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -3253,13 +3307,13 @@
         <v>40</v>
       </c>
       <c r="D127" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E127" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F127" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -3270,13 +3324,13 @@
         <v>41</v>
       </c>
       <c r="D128" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E128" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F128" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -3287,13 +3341,13 @@
         <v>42</v>
       </c>
       <c r="D129" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E129" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F129" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -3304,13 +3358,13 @@
         <v>43</v>
       </c>
       <c r="D130" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E130" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F130" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -3321,13 +3375,13 @@
         <v>44</v>
       </c>
       <c r="D131" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E131" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F131" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -3338,13 +3392,13 @@
         <v>45</v>
       </c>
       <c r="D132" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E132" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F132" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -3355,13 +3409,13 @@
         <v>46</v>
       </c>
       <c r="D133" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E133" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F133" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -3372,13 +3426,13 @@
         <v>48</v>
       </c>
       <c r="D134" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E134" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F134" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -3389,13 +3443,13 @@
         <v>49</v>
       </c>
       <c r="D135" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E135" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F135" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -3406,13 +3460,13 @@
         <v>50</v>
       </c>
       <c r="D136" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E136" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F136" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -3423,13 +3477,13 @@
         <v>51</v>
       </c>
       <c r="D137" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E137" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F137" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -3440,13 +3494,13 @@
         <v>52</v>
       </c>
       <c r="D138" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E138" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F138" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -3457,13 +3511,13 @@
         <v>53</v>
       </c>
       <c r="D139" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E139" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F139" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3725,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3746,58 +3800,122 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3807,10 +3925,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3825,10 +3943,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Messing around with some modelling - to be removed.
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99928DCD-C62C-416D-9114-F827FA361642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF703FA-F57A-4534-9C7A-FBC03A649A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="-25920" windowWidth="23232" windowHeight="25296" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
-    <sheet name="Groups" sheetId="2" r:id="rId2"/>
-    <sheet name="Transformations" sheetId="3" r:id="rId3"/>
-    <sheet name="Views" sheetId="4" r:id="rId4"/>
+    <sheet name="ID" sheetId="5" r:id="rId2"/>
+    <sheet name="Groups" sheetId="2" r:id="rId3"/>
+    <sheet name="Transformations" sheetId="3" r:id="rId4"/>
+    <sheet name="Models" sheetId="7" r:id="rId5"/>
+    <sheet name="Views" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="209">
   <si>
     <t>Plate</t>
   </si>
@@ -500,9 +502,6 @@
     <t>comb</t>
   </si>
   <si>
-    <t>combine_samples,plate_01_time.flo</t>
-  </si>
-  <si>
     <t>flo_od</t>
   </si>
   <si>
@@ -603,6 +602,72 @@
   </si>
   <si>
     <t>700,(558,602),(558,602[2])</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>558,602</t>
+  </si>
+  <si>
+    <t>flo</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>Current ID</t>
+  </si>
+  <si>
+    <t>Replaced ID</t>
+  </si>
+  <si>
+    <t>combine_samples_flo,plate_01_time.flo</t>
+  </si>
+  <si>
+    <t>Solver</t>
+  </si>
+  <si>
+    <t>Fit</t>
+  </si>
+  <si>
+    <t>Vary</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>ODE</t>
+  </si>
+  <si>
+    <t>Rodas4P</t>
+  </si>
+  <si>
+    <t>(k,1:4:0.5)</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>k,a--&gt;b</t>
+  </si>
+  <si>
+    <t>k=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a=1, b=1 </t>
+  </si>
+  <si>
+    <t>(a,sg1)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -644,9 +709,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1021,10 +1087,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1748,6 +1814,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B2676-373C-45A2-B753-09761E8A63AC}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -1998,12 +2106,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,122 +2129,122 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" t="s">
         <v>181</v>
-      </c>
-      <c r="B14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2144,12 +2252,90 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AEE18E-F6A9-4B87-A075-2291935DF4B5}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2167,15 +2353,15 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update - some data loss due to improper copying but none of the key files.
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\EEBio\eebio-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF703FA-F57A-4534-9C7A-FBC03A649A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC8E79E-52D8-42B3-8A87-79675AF35EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="4" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="212">
   <si>
     <t>Plate</t>
   </si>
@@ -616,12 +616,6 @@
     <t>OD</t>
   </si>
   <si>
-    <t>Current ID</t>
-  </si>
-  <si>
-    <t>Replaced ID</t>
-  </si>
-  <si>
     <t>combine_samples_flo,plate_01_time.flo</t>
   </si>
   <si>
@@ -668,6 +662,21 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>flow_cy</t>
+  </si>
+  <si>
+    <t>flow_cyt</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>process_fcs("plate_02",["FSC-A","SSC-A"],["BL1-H"])</t>
   </si>
 </sst>
 </file>
@@ -1818,7 +1827,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,10 +1837,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2108,10 +2117,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,6 +2256,14 @@
         <v>182</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2256,7 +2273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AEE18E-F6A9-4B87-A075-2291935DF4B5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2272,57 +2289,57 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" t="s">
         <v>194</v>
-      </c>
-      <c r="G1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H1" t="s">
-        <v>195</v>
-      </c>
-      <c r="I1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" t="s">
         <v>197</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" t="s">
-        <v>199</v>
       </c>
       <c r="G2">
         <v>10000</v>
       </c>
       <c r="H2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2332,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,7 +2370,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2362,6 +2379,14 @@
       </c>
       <c r="B3" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the command line version. needs documentation.
</commit_message>
<xml_diff>
--- a/ESM_input_test.xlsx
+++ b/ESM_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micha\eebio-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC8E79E-52D8-42B3-8A87-79675AF35EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD7BECA-33A4-495F-9F59-8FC8D0A33CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="4536" yWindow="4536" windowWidth="23040" windowHeight="13560" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="215">
   <si>
     <t>Plate</t>
   </si>
@@ -677,6 +677,15 @@
   </si>
   <si>
     <t>process_fcs("plate_02",["FSC-A","SSC-A"],["BL1-H"])</t>
+  </si>
+  <si>
+    <t>test_doub</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>doubling_time(combine_samples_od, plate_01_time.OD;max_od=0.2)</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2126,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -2262,6 +2271,14 @@
       </c>
       <c r="B17" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2349,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AD15BF-AC00-4821-ADC5-28168A3A0A78}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,6 +2406,14 @@
         <v>208</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>